<commit_message>
feat: Add delivery package
</commit_message>
<xml_diff>
--- a/cli/orders-ecom.xlsx
+++ b/cli/orders-ecom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookair/Desktop/JoCode/E-Com/Automation/cli/cli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookair/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93E7F29-4A90-5342-A45F-94D417D7B102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC71698E-7C59-7644-AFBF-DB50596BCB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{0F18FA96-B28C-F540-B200-7F2C14E5EC49}"/>
+    <workbookView xWindow="4300" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{0F18FA96-B28C-F540-B200-7F2C14E5EC49}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>N</t>
   </si>
@@ -82,7 +82,19 @@
     <t>Koumassi Quartier Divo</t>
   </si>
   <si>
-    <t>Chapelet</t>
+    <t>Attâche câbles à crochet et à boucle</t>
+  </si>
+  <si>
+    <t>HARRY POTTER</t>
+  </si>
+  <si>
+    <t>SATORU GOJO</t>
+  </si>
+  <si>
+    <t>JOCODE DEV</t>
+  </si>
+  <si>
+    <t>Koumassi Quartier Divo carrefour canniveau - premier carrefour à gauche</t>
   </si>
 </sst>
 </file>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D855648-AD52-A544-96D3-A160728CF516}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="D10" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,6 +459,7 @@
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -600,10 +613,82 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>5000</v>
       </c>
     </row>

</xml_diff>